<commit_message>
converted xcel files to pdf
</commit_message>
<xml_diff>
--- a/documentatie/CRPR management - AO - 2017 - ict college.xlsx
+++ b/documentatie/CRPR management - AO - 2017 - ict college.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proftaak2\documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\Semester 4\web\proftaak2\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{60469DED-F0C1-4011-B256-F859CCEC131C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BC0B3A86-8AE8-4458-8816-10E223829E4E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
     <definedName name="TSA_afspraken">[1]bronteksten!#REF!</definedName>
     <definedName name="TSAnr">[1]bronteksten!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,12 +45,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>hierboven aanvullen</t>
-  </si>
-  <si>
-    <t>nieuw</t>
   </si>
   <si>
     <t>afgewerkt</t>
@@ -99,9 +96,6 @@
     <t>Oude library had niet alle functionaliteiten die we nodig hebben</t>
   </si>
   <si>
-    <t>Overgestapt van Bootstrap naar MaterializeCSS</t>
-  </si>
-  <si>
     <t>Materialize ziet er mooier uit dan bootstrap en heeft een aantal erg handige functies</t>
   </si>
   <si>
@@ -118,6 +112,10 @@
   </si>
   <si>
     <t>DBOS/RBRO</t>
+  </si>
+  <si>
+    <t>Overgestapt van Bootstrap 
+naar MaterializeCSS</t>
   </si>
 </sst>
 </file>
@@ -172,7 +170,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -186,17 +184,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color auto="1"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="hair">
-        <color auto="1"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="hair">
-        <color auto="1"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="hair">
-        <color auto="1"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -204,55 +202,68 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="76">
     <dxf>
@@ -1171,845 +1182,202 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Blad1"/>
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="4" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="10.6640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="68.44140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16" style="1" customWidth="1"/>
-    <col min="9" max="9" width="41.109375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="10.6640625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.77734375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="16" style="3" customWidth="1"/>
+    <col min="9" max="9" width="41.109375" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="F1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="15" t="s">
         <v>4</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3">
+      <c r="C2" s="18"/>
+      <c r="D2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="20">
         <v>43448</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="21" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
+      <c r="C3" s="18"/>
+      <c r="D3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="20">
         <v>43451</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>22</v>
+      <c r="I3" s="21" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="18">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="C4" s="18"/>
+      <c r="D4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="20">
         <v>43434</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>18</v>
+      <c r="G4" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="18">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="C5" s="18"/>
+      <c r="D5" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="20">
         <v>43441</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>20</v>
+      <c r="G5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="B6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="3">
+      <c r="C6" s="18"/>
+      <c r="D6" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="20">
         <v>43476</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="G6" s="21" t="s">
         <v>13</v>
       </c>
+      <c r="H6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I28" s="10"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G34" s="11"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>9</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>12</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>13</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>14</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>15</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>16</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <v>18</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
-        <v>19</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
-        <v>20</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
-        <v>21</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
-        <v>22</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
-        <v>23</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
-        <v>24</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
-        <v>25</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
-        <v>26</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="11"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
-        <v>27</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
-        <v>28</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
-        <v>29</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
-        <v>30</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
-        <v>31</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="4">
-        <v>32</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
-        <v>33</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
-        <v>34</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
-        <v>35</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
-        <v>36</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
-        <v>37</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
-        <v>38</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
-        <v>39</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
-        <v>40</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
-        <v>41</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
-        <v>42</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
-        <v>43</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
-        <v>44</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="4">
-        <v>45</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
-        <v>46</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="4">
-        <v>47</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="4">
-        <v>48</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="4">
-        <v>49</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="4">
-        <v>50</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="4">
-        <v>51</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="4">
-        <v>52</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="4">
-        <v>53</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="4">
-        <v>54</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="4">
-        <v>55</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="4">
-        <v>56</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="4">
-        <v>57</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="4">
-        <v>58</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="4">
-        <v>59</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="4">
-        <v>60</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="4">
-        <v>61</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="4">
-        <v>62</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="4">
-        <v>63</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="4">
-        <v>64</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="4">
-        <v>65</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="4">
-        <v>66</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="4">
-        <v>67</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="4">
-        <v>68</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="4">
-        <v>69</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="4">
-        <v>70</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="4">
-        <v>71</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="4">
-        <v>72</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="4">
-        <v>73</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="4">
-        <v>74</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="4">
-        <v>75</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="4">
-        <v>76</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="4">
-        <v>77</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="4">
-        <v>78</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="4">
-        <v>79</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="4">
-        <v>80</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="4">
-        <v>81</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="4">
-        <v>82</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="4">
-        <v>83</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="4">
-        <v>84</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="4">
-        <v>85</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="4">
-        <v>86</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="4">
-        <v>87</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="7"/>
-      <c r="G91" s="5"/>
-      <c r="H91" s="6"/>
-      <c r="I91" s="5"/>
+    <row r="45" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="I45" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I54" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="D91:E1048576 E90 E5 E11:E39 D6:E9 D11:D64 D1:E2 E3">
+  <conditionalFormatting sqref="E90 E5 E11:E39 D11:D64 D1:E2 E3 D92:E1048576 D6:E9">
     <cfRule type="cellIs" dxfId="75" priority="98" operator="equal">
       <formula>"niet nodig"</formula>
     </cfRule>
@@ -2274,6 +1642,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>